<commit_message>
Complete Georgia (GA) scraper - 25 staff members
</commit_message>
<xml_diff>
--- a/Desktop/Claude Code Projects/State MEPs/state_meps.xlsx
+++ b/Desktop/Claude Code Projects/State MEPs/state_meps.xlsx
@@ -1727,13 +1727,11 @@
           <t>954-253-7289</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
           <t>kaitlin.centonze@floridamakes.com</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1751,7 +1749,6 @@
           <t>315-350-6656</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>connor.hlywa@floridamakes.com</t>
@@ -1779,7 +1776,6 @@
           <t>850-699-5201</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
           <t>beth.maraman@floridamakes.com</t>
@@ -1807,7 +1803,6 @@
           <t>561-634-1334</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
           <t>amanda.marcusky@floridamakes.com</t>
@@ -1835,7 +1830,6 @@
           <t>904-728-2470</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
           <t>amanda.starling@floridamakes.com</t>
@@ -1863,7 +1857,6 @@
           <t>347-362-7685</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
           <t>mariely.velez@floridamakes.com</t>
@@ -1891,7 +1884,6 @@
           <t>407-470-0476</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
           <t>patricia.velez@floridamakes.com</t>
@@ -1914,7 +1906,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1965,6 +1957,406 @@
           <t>https://gamep.org/meet-the-gamep-team/</t>
         </is>
       </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Tim Israel</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Director</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cassia Baker</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Project Manager, Cybersecurity</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Michael Barker</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Project Manager, Cybersecurity</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Sam Darwin</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Project Manager, Process Improvement</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Sandra Enciso</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Project Manager, Energy and Sustainability</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Alfred Gardner</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Project Manager, Human Resources</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Bogna Grabicka</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Project Manager, Safety and Sustainability</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Kelly Grissom</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Project Manager, Energy and Sustainability</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Andy Helm</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Project Manager, Strategy and Leadership Development</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Dean Hettenbach</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Project Manager, Supply Chain and Technology</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Katie Hines</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Project Manager, Process Improvement</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Andrea Hines</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Project Manager, Food and Beverage</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Andrew Krejci</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Project Manager, Technology</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Ben Cheeks</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Region Manager, Coastal Georgia</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Jason Clarke</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Region Manager, Northeast Georgia</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Hank Hobbs</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Region Manager, South Georgia</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Paul LaVigna</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Region Manager, South Metro Atlanta</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Jay Boudreaux</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Senior Program and Operations Manager</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Anna Cali</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Instructional Systems Designer</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Jasmyn Green</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Program and Operations Manager</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Raine Hyde</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Marketing Strategist</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Megan Johnson</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Marketing Manager, Outreach</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Ieasha Jones</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Special Events</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Amber Kasselman</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Marketing Manager</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Caley Landau</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Marketing Strategist</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Complete Hawaii (HI) scraper - 13 staff members
</commit_message>
<xml_diff>
--- a/Desktop/Claude Code Projects/State MEPs/state_meps.xlsx
+++ b/Desktop/Claude Code Projects/State MEPs/state_meps.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="9" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="11" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Master List" sheetId="1" state="visible" r:id="rId1"/>
@@ -1657,7 +1657,7 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -1906,13 +1906,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="17" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="51.5703125" bestFit="1" customWidth="1" min="2" max="2"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -1969,10 +1973,6 @@
           <t>Director</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1985,10 +1985,6 @@
           <t>Project Manager, Cybersecurity</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2001,10 +1997,6 @@
           <t>Project Manager, Cybersecurity</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2017,10 +2009,6 @@
           <t>Project Manager, Process Improvement</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2033,10 +2021,6 @@
           <t>Project Manager, Energy and Sustainability</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2049,10 +2033,6 @@
           <t>Project Manager, Human Resources</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2065,10 +2045,6 @@
           <t>Project Manager, Safety and Sustainability</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2081,10 +2057,6 @@
           <t>Project Manager, Energy and Sustainability</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2097,10 +2069,6 @@
           <t>Project Manager, Strategy and Leadership Development</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2113,10 +2081,6 @@
           <t>Project Manager, Supply Chain and Technology</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2129,10 +2093,6 @@
           <t>Project Manager, Process Improvement</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2145,10 +2105,6 @@
           <t>Project Manager, Food and Beverage</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2161,10 +2117,6 @@
           <t>Project Manager, Technology</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2177,10 +2129,6 @@
           <t>Region Manager, Coastal Georgia</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2193,10 +2141,6 @@
           <t>Region Manager, Northeast Georgia</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2209,10 +2153,6 @@
           <t>Region Manager, South Georgia</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2225,10 +2165,6 @@
           <t>Region Manager, South Metro Atlanta</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2241,10 +2177,6 @@
           <t>Senior Program and Operations Manager</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2257,10 +2189,6 @@
           <t>Instructional Systems Designer</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2273,10 +2201,6 @@
           <t>Program and Operations Manager</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2289,10 +2213,6 @@
           <t>Marketing Strategist</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2305,10 +2225,6 @@
           <t>Marketing Manager, Outreach</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2321,10 +2237,6 @@
           <t>Special Events</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2337,10 +2249,6 @@
           <t>Marketing Manager</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2353,10 +2261,6 @@
           <t>Marketing Strategist</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2369,9 +2273,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2420,6 +2324,214 @@
           <t>https://www.htdc.org/our-team/</t>
         </is>
       </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Trung Lam</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Executive Director &amp; CEO / Acting MEP Center Director</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Matthew Kobayashi</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Project Development Manager</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Sandi Kanemori</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Sr. Economic Program Manager</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Umma Berkelman</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Economic Development Specialist</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Cindy Matsuki</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Economic Development Specialist - HSBIR</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Karlton Tomomitsu</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Economic Development Specialist</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Dave Molinaro</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>HCATT Director</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Kristy Carpio</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>HCATT Project Manager</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Tuan La</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>HI-CAP Manager</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Wayne Layugan</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Program Manager</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Wendy Oshiro</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Project Manager</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Ray Gomez</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Chief Financial Officer</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Stephanie Yuu-Sato</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Contracts &amp; Project Manager</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>